<commit_message>
update arrival data with 2024
</commit_message>
<xml_diff>
--- a/ArrivalData.xlsx
+++ b/ArrivalData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holtz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EC0D248-03AC-2543-8BBD-88D946C7096A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF060D8-93D6-1B40-87B6-9CA11DF9A3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29860" yWindow="2820" windowWidth="28040" windowHeight="16540" xr2:uid="{8D11DE6F-C818-8543-AF20-356AD556DC00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Caballo</t>
   </si>
@@ -44,22 +44,38 @@
     <t>Leasburg</t>
   </si>
   <si>
-    <t>6/2/22/9:33</t>
+    <t>Picacho</t>
   </si>
   <si>
-    <t>Picacho</t>
+    <t>YEAR/LOCATION</t>
+  </si>
+  <si>
+    <t>Date/time</t>
+  </si>
+  <si>
+    <t>flow/height</t>
+  </si>
+  <si>
+    <t>NOTES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -83,9 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,23 +438,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1BF89A-83BA-9E4E-99C2-FBD69949F886}">
-  <dimension ref="A3:C22"/>
+  <dimension ref="A2:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -447,7 +481,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>44347.376388888886</v>
       </c>
@@ -455,7 +489,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -466,7 +500,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>44348.545138888891</v>
       </c>
@@ -474,9 +508,9 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1">
         <v>44349.17083333333</v>
@@ -485,15 +519,15 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>2022</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -504,7 +538,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>44713.293055555558</v>
       </c>
@@ -512,18 +546,18 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>2</v>
+      <c r="B13" s="1">
+        <v>44714.397916666669</v>
       </c>
       <c r="C13">
         <v>374</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>44714.502083333333</v>
       </c>
@@ -531,9 +565,9 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1">
         <v>44715.085416666669</v>
@@ -542,11 +576,11 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>2023</v>
       </c>
     </row>
@@ -590,13 +624,67 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" s="1">
         <v>45059.688888888886</v>
       </c>
       <c r="C22">
         <v>4.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45359.354166666664</v>
+      </c>
+      <c r="C25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>45359.395833333336</v>
+      </c>
+      <c r="C26">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45360.271527777775</v>
+      </c>
+      <c r="C27">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>45360.334027777775</v>
+      </c>
+      <c r="C28">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3">
+        <v>45360.750694444447</v>
+      </c>
+      <c r="C29">
+        <v>4.3600000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>